<commit_message>
Updates to ALLURE Epic Table
</commit_message>
<xml_diff>
--- a/EPIC Allure Coverage/IH_Epic_Summary_XL_cf_v1-0_240225.xlsx
+++ b/EPIC Allure Coverage/IH_Epic_Summary_XL_cf_v1-0_240225.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,11 +472,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NVHUB-5339: CDS UI Component Library - Migration</t>
+          <t>INVHUB-1018: User/System Preferences</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
@@ -502,11 +502,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INVHUB-18: Authentication and Login</t>
+          <t>INVHUB-1035: Sensa Copilot for Investigators GA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -518,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>100</v>
@@ -532,11 +532,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INVHUB-4521: NFR - Security</t>
+          <t>INVHUB-10821: Filtering on transactions</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
         <v>100</v>
@@ -562,11 +562,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INVHUB-13905: (Phase 2) Workflow Actions mgmt</t>
+          <t>INVHUB-1180: Sensa Copilot enhancements/support(Q1)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>100</v>
@@ -622,11 +622,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INVHUB-5339: CDS UI Component Library - Migration</t>
+          <t>INVHUB-13905: (Phase 2) Workflow Actions mgmt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G7" t="n">
         <v>100</v>
@@ -652,11 +652,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>INVHUB-9920: Tag Category (workflow)</t>
+          <t>INVHUB-18: Authentication and Login</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
         <v>100</v>
@@ -682,11 +682,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INVHUB-8565: Refinements to event/audit log</t>
+          <t>INVHUB-4521: NFR - Security</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
         <v>100</v>
@@ -712,7 +712,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>INVHUB-7539: Tags Management</t>
+          <t>INVHUB-5339: CDS UI Component Library - Migration</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -742,11 +742,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>INVHUB-1180: Sensa Copilot enhancements/support(Q1)</t>
+          <t>INVHUB-7539: Tags Management</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
         <v>100</v>
@@ -772,26 +772,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INVHUB-9919: (Phase 3) Workflow - Decision making and multi level workflows</t>
+          <t>INVHUB-8565: Refinements to event/audit log</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>96.3</v>
+        <v>100</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -802,11 +802,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INVHUB-10821: Filtering on transactions</t>
+          <t>INVHUB-9173: Abanca Technical POC</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
         <v>100</v>
@@ -832,11 +832,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INVHUB-1035: Sensa Copilot for Investigators GA</t>
+          <t>INVHUB-9920: Tag Category (workflow)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G14" t="n">
         <v>100</v>
@@ -862,11 +862,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>INVHUB-1018: User/System Preferences</t>
+          <t>NVHUB-5339: CDS UI Component Library - Migration</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
         <v>100</v>
@@ -892,26 +892,26 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>API Testing: GraphQL</t>
+          <t>INVHUB-9369: IH : Language dropdown to generate Narrative  - No EPIC Tagged</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>163</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>95.88</v>
+        <v>100</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -922,14 +922,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>INVHUB-9173: Abanca Technical POC</t>
+          <t>INVHUB-2377: Roles Management Q1</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -938,10 +938,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="G17" t="n">
-        <v>100</v>
+        <v>96.88</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -952,26 +952,26 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>INVHUB-2377: Roles Management Q1</t>
+          <t>INVHUB-9919: (Phase 3) Workflow - Decision making and multi level workflows</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="G18" t="n">
-        <v>96.88</v>
+        <v>96.3</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -982,30 +982,30 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>INVHUB-9920: Maintenance of Tags and Tag Categories</t>
+          <t>API Testing: GraphQL</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="C19" t="n">
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="G19" t="n">
-        <v>84.20999999999999</v>
+        <v>95.88</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Maintenance Advised</t>
+          <t>Acceptable</t>
         </is>
       </c>
     </row>
@@ -1042,26 +1042,26 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>INVHUB-3120: Workflows -Manager creation of Actions / map to teams</t>
+          <t>INVHUB-2452: Enhancements to the investigator experience</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F21" t="n">
-        <v>96</v>
+        <v>214</v>
       </c>
       <c r="G21" t="n">
-        <v>84.38</v>
+        <v>90.19</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1072,26 +1072,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>INVHUB-2452: Enhancements to the investigator experience</t>
+          <t>INVHUB-2168: Teams Management - Q1</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>214</v>
+        <v>8</v>
       </c>
       <c r="G22" t="n">
-        <v>90.19</v>
+        <v>87.5</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1102,26 +1102,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>API Testing</t>
+          <t>INVHUB-3120: Workflows -Manager creation of Actions / map to teams</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="C23" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>239</v>
+        <v>96</v>
       </c>
       <c r="G23" t="n">
-        <v>83.68000000000001</v>
+        <v>84.38</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1132,14 +1132,14 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>INVHUB-2168: Teams Management - Q1</t>
+          <t>INVHUB-9920: Maintenance of Tags and Tag Categories</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1148,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="G24" t="n">
-        <v>87.5</v>
+        <v>84.20999999999999</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1162,56 +1162,56 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>INVHUB-1047: Subject Centric Investigation - TM</t>
+          <t>API Testing</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
-        <v>8</v>
+        <v>239</v>
       </c>
       <c r="G25" t="n">
-        <v>62.5</v>
+        <v>83.68000000000001</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Review Required</t>
+          <t>Maintenance Advised</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>INVHUB-11621: Provide detailed analysis at the individual detection level</t>
+          <t>INVHUB-8981: Narrative contribution and UI view</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C26" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>47.37</v>
+        <v>75</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1222,26 +1222,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>INVHUB-966: Open Investigations queue/list (GA)</t>
+          <t>INVHUB-8114: Authentication</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C27" t="n">
+        <v>7</v>
+      </c>
+      <c r="D27" t="n">
         <v>4</v>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>73.17</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1252,26 +1252,26 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>INVHUB-11811: Prefill transactions on the transaction tab</t>
+          <t>INVHUB-126: Entity Centric Investigation (Subject Details) (MVP)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C28" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="G28" t="n">
-        <v>52.17</v>
+        <v>65.22</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1282,26 +1282,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INVHUB-8981: Narrative contribution and UI view</t>
+          <t>INVHUB-1047: Subject Centric Investigation - TM</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G29" t="n">
-        <v>75</v>
+        <v>62.5</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1312,14 +1312,14 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>INVHUB-11963: Copilot: Add  some  more complex and standard  queries for Transactions</t>
+          <t>INVHUB-11811: Prefill transactions on the transaction tab</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1328,10 +1328,10 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G30" t="n">
-        <v>38.46</v>
+        <v>52.17</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1342,26 +1342,26 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>INVHUB-8114: Authentication</t>
+          <t>INVHUB-157: Assign (Reassign) and drill down (GA)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>73.17</v>
+        <v>50</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1372,14 +1372,14 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>INVHUB-290: Teams Management</t>
+          <t>INVHUB-2136: Subject Centric Investigation(Q1)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1388,10 +1388,10 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>43.75</v>
+        <v>50</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1402,26 +1402,26 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>INVHUB-7367: IH Bugs</t>
+          <t>INVHUB-11621: Provide detailed analysis at the individual detection level</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C33" t="n">
+        <v>7</v>
+      </c>
+      <c r="D33" t="n">
         <v>2</v>
       </c>
-      <c r="D33" t="n">
-        <v>5</v>
-      </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F33" t="n">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="G33" t="n">
-        <v>12.5</v>
+        <v>47.37</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -1432,26 +1432,26 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INVHUB-5: Open Investigations List</t>
+          <t>Test Cases Not Tagged</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F34" t="n">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>44.85</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1462,11 +1462,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>INVHUB-13708: Transaction Ingestion Phase 1</t>
+          <t>INVHUB-290: Teams Management</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C35" t="n">
         <v>9</v>
@@ -1478,10 +1478,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G35" t="n">
-        <v>10</v>
+        <v>43.75</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1492,26 +1492,26 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>INVHUB-4976: Data Access - Q2</t>
+          <t>INVHUB-13: Menu and User Administration</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="G36" t="n">
-        <v>11.11</v>
+        <v>40</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -1522,26 +1522,26 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>INVHUB-13: Menu and User Administration</t>
+          <t>INVHUB-11963: Copilot: Add  some  more complex and standard  queries for Transactions</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G37" t="n">
-        <v>40</v>
+        <v>38.46</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -1552,26 +1552,26 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>INVHUB-157: Assign (Reassign) and drill down (GA)</t>
+          <t>INVHUB-7367: IH Bugs</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G38" t="n">
-        <v>50</v>
+        <v>12.5</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1582,26 +1582,26 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>INVHUB-171: Data Access - GA</t>
+          <t>INVHUB-4976: Data Access - Q2</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1612,14 +1612,14 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>INVHUB-2136: Subject Centric Investigation(Q1)</t>
+          <t>INVHUB-13708: Transaction Ingestion Phase 1</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
@@ -1628,10 +1628,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G40" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1642,26 +1642,26 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>INVHUB-126: Entity Centric Investigation (Subject Details) (MVP)</t>
+          <t>INVHUB-171: Data Access - GA</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="G41" t="n">
-        <v>65.22</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -1672,26 +1672,146 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>INVHUB-5: Open Investigations List</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Review Required</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>INVHUB-966: Open Investigations queue/list (GA)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Review Required</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>INVHUB-135: Dual browser capability - No EPIC Tagged</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Review Required</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>INVHUB-8203: Remove Sensa Roles: Investigation Hub Roles to become the only Roles available - No EPIC Tagged</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Review Required</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>990</v>
-      </c>
-      <c r="C42" t="n">
-        <v>138</v>
-      </c>
-      <c r="D42" t="n">
-        <v>73</v>
-      </c>
-      <c r="E42" t="n">
-        <v>52</v>
-      </c>
-      <c r="F42" t="n">
-        <v>1253</v>
-      </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="B46" t="n">
+        <v>1066</v>
+      </c>
+      <c r="C46" t="n">
+        <v>170</v>
+      </c>
+      <c r="D46" t="n">
+        <v>122</v>
+      </c>
+      <c r="E46" t="n">
+        <v>66</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1424</v>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>